<commit_message>
updated Sprint Backlog and Documentation
</commit_message>
<xml_diff>
--- a/D3/Sprint #2 - Sprint Backlog.xlsx
+++ b/D3/Sprint #2 - Sprint Backlog.xlsx
@@ -194,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -233,12 +233,6 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -313,7 +307,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,7 +321,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -359,6 +352,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -741,23 +740,52 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="76.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="3" max="5" width="9" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18">
+        <v>42305</v>
+      </c>
+      <c r="D1" s="18">
+        <v>42306</v>
+      </c>
+      <c r="E1" s="18">
+        <v>42307</v>
+      </c>
+      <c r="F1" s="18">
+        <v>42310</v>
+      </c>
+      <c r="G1" s="18">
+        <v>42311</v>
+      </c>
+      <c r="H1" s="19">
+        <v>42312</v>
+      </c>
+      <c r="I1" s="18">
+        <v>42313</v>
+      </c>
+      <c r="J1" s="18">
+        <v>42314</v>
+      </c>
+      <c r="K1" s="18">
+        <v>42317</v>
+      </c>
+      <c r="L1" s="18">
+        <v>42318</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="14.45" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -801,10 +829,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="2">
@@ -843,11 +871,11 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="2">
@@ -856,7 +884,7 @@
       <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>0</v>
       </c>
       <c r="G4" s="2">
@@ -883,8 +911,8 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="17"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2">
@@ -923,8 +951,8 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="17"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="2">
@@ -954,7 +982,7 @@
       <c r="K6" s="2">
         <v>0</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>0.5</v>
       </c>
       <c r="N6">
@@ -963,8 +991,8 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="17"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2">
@@ -1003,8 +1031,8 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="17"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2">
@@ -1043,8 +1071,8 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="17"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2">
@@ -1083,29 +1111,29 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>1</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>1</v>
       </c>
-      <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="10">
         <v>0</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="2">
-        <v>0</v>
+      <c r="I10" s="9">
+        <v>1.5</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
@@ -1113,12 +1141,12 @@
       <c r="K10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <v>0.5</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1126,60 +1154,60 @@
         <v>13</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <f t="shared" ref="C12:L12" si="1">SUM(C3:C10)</f>
         <v>2</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G12" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="14">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="M12" s="2"/>
-      <c r="N12" s="14">
+      <c r="N12" s="13">
         <f>B14</f>
-        <v>6</v>
-      </c>
-      <c r="O12" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="O12" s="11"/>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <f>SUM(N3:N10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
change in sprint backlog
</commit_message>
<xml_diff>
--- a/D3/Sprint #2 - Sprint Backlog.xlsx
+++ b/D3/Sprint #2 - Sprint Backlog.xlsx
@@ -191,17 +191,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="10">
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -228,12 +222,6 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="53"/>
-      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -312,31 +300,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -345,25 +333,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -371,14 +359,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -754,7 +742,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -877,11 +865,11 @@
         <v>0</v>
       </c>
       <c r="L3" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N10" si="0">SUM(C3:L3)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:14">
@@ -1206,12 +1194,12 @@
       </c>
       <c r="L12" s="15">
         <f>SUM(L3:L10)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="15">
         <f>B14</f>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="O12" s="20"/>
     </row>
@@ -1221,7 +1209,7 @@
       </c>
       <c r="B14" s="18">
         <f>SUM(N3:N10)</f>
-        <v>9.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customHeight="1"/>

</xml_diff>